<commit_message>
some more problems on tree
</commit_message>
<xml_diff>
--- a/Articles/problem set.xlsx
+++ b/Articles/problem set.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnpat\OneDrive\Documents\Graph Problems\Articles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BCB5A64-470B-4459-9E03-686ECF2EF9DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2FB271-054D-4F85-9F5F-0520523A220C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4690" yWindow="1740" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="243">
   <si>
     <t>Tag</t>
   </si>
@@ -704,6 +703,57 @@
   </si>
   <si>
     <t>(Booking app,google earth,chatting app)</t>
+  </si>
+  <si>
+    <t>Insertion in BST</t>
+  </si>
+  <si>
+    <t>Search given key in BST</t>
+  </si>
+  <si>
+    <t>Deletion from BST</t>
+  </si>
+  <si>
+    <t>Construct balanced BST from given keys</t>
+  </si>
+  <si>
+    <t>Determine if given Binary tree is a BST or not</t>
+  </si>
+  <si>
+    <t>check if given keys represent same bst without building bst</t>
+  </si>
+  <si>
+    <t>find inorder predecessor for given key in a bst</t>
+  </si>
+  <si>
+    <t>find lowest common ansector of two nodes in bst</t>
+  </si>
+  <si>
+    <t>kth smallest and kth largest element in BST</t>
+  </si>
+  <si>
+    <t>fllor and ciel in bst</t>
+  </si>
+  <si>
+    <t>find optimal cost to construct bst</t>
+  </si>
+  <si>
+    <t>tree to bst while maintiang original strucute</t>
+  </si>
+  <si>
+    <t>remove nodes from bst that have key outside a given a range</t>
+  </si>
+  <si>
+    <t>find a pair with given sum in bst</t>
+  </si>
+  <si>
+    <t>inorder sucessor of bst</t>
+  </si>
+  <si>
+    <t>fix a binary tree that is onle one swap away from becoming a bst</t>
+  </si>
+  <si>
+    <t>update every key in bst to contain sum of all greater keys</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D216"/>
+  <dimension ref="A1:D233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="A217" sqref="A217"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2169,6 +2219,91 @@
         <v>225</v>
       </c>
     </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>242</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
created a folder to track 500 more quora dsa problems, started with d
</commit_message>
<xml_diff>
--- a/Articles/problem set.xlsx
+++ b/Articles/problem set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnpat\OneDrive\Documents\Graph Problems\Articles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2FB271-054D-4F85-9F5F-0520523A220C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A241569E-3E5F-458A-B13C-B7515D449A6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4690" yWindow="1740" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="244">
   <si>
     <t>Tag</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>update every key in bst to contain sum of all greater keys</t>
+  </si>
+  <si>
+    <t>Knapsack Problem with restriction that no two consecutive elements can be choosen</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D233"/>
+  <dimension ref="A1:D234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="A235" sqref="A235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2304,6 +2307,11 @@
         <v>242</v>
       </c>
     </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>